<commit_message>
fix update perhitungan btn indonesia
</commit_message>
<xml_diff>
--- a/Data/Data_Negatif.xlsx
+++ b/Data/Data_Negatif.xlsx
@@ -957,13 +957,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="23.4285714285714" customWidth="1"/>
     <col min="2" max="2" width="20.8571428571429" customWidth="1"/>
@@ -984,7 +984,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>10000000</v>
+        <v>2300000</v>
       </c>
       <c r="B2">
         <v>65000000</v>
@@ -995,7 +995,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>20000000</v>
+        <v>3500000</v>
       </c>
       <c r="B3">
         <v>105500000</v>
@@ -1006,57 +1006,13 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>30000000</v>
+        <v>3500000</v>
       </c>
       <c r="B4">
         <v>200500000</v>
       </c>
       <c r="C4">
         <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>40000000</v>
-      </c>
-      <c r="B5">
-        <v>200500000</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>50000000</v>
-      </c>
-      <c r="B6">
-        <v>2000500000</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>60000000</v>
-      </c>
-      <c r="B7">
-        <v>32000500000</v>
-      </c>
-      <c r="C7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>70000000</v>
-      </c>
-      <c r="B8">
-        <v>3232500000</v>
-      </c>
-      <c r="C8">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>